<commit_message>
minor tweeks to some of the tests
</commit_message>
<xml_diff>
--- a/src/RegressionTests/Katalon/inputFiles/TEST_insertHomologuesThroughPipeline.xlsx
+++ b/src/RegressionTests/Katalon/inputFiles/TEST_insertHomologuesThroughPipeline.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Documents\HRInternetConsulting\Clients\FHCRC\Tachyon\src\selenium\inputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Documents\HRInternetConsulting\Clients\FHCRC\Tachyon\src\RegressionTests\Katalon\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -89,43 +89,43 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>TESTTTTTSCFKRNRQCKGSFLKSACCEGLKCVNGRCT</t>
-  </si>
-  <si>
-    <t>TESTTTTTDCCFSSSCRCNLWGSNCQCQRMGLFQKWGASPL</t>
-  </si>
-  <si>
-    <t>TESTTTTTCSPPGFFCQTDDDCCFTKLFRCLEIVGRCVKRNVTVASTTALPTNSINL</t>
-  </si>
-  <si>
-    <t>TESTTTTTSAIPHCSPWRCQQECLFKNFMKGECIQLQCVCSQKIGGIRP</t>
-  </si>
-  <si>
-    <t>TESTTTTTDCTGWMGGCDPSKTGECCSGYVCSYKYPWCRYDLF</t>
-  </si>
-  <si>
-    <t>TESTTTTTVSFCLLPIVPGPCTQYVIRYAFQPSISACRRFTFGGCEGNDNNFMTRRDCEHYCEELL</t>
-  </si>
-  <si>
-    <t>TESTTTTTYKGCRRLGSKCHPTLKPCCSALTCKPIDGDNGECVE</t>
-  </si>
-  <si>
-    <t>TESTTTTTYCLGSGEECGKFDDCCSLTCMSNGECA</t>
-  </si>
-  <si>
-    <t>TESTTTTTCSPPGAVCDSFNNCCTGFMCNPWAKRCTRGFFDRIPLKTKKYNFSNQIMNEE</t>
-  </si>
-  <si>
-    <t>TESTTTTTAPNSMDSCFDLAQFCVMSEQCCPGLQCSSYAAKCIPIYIYN</t>
-  </si>
-  <si>
-    <t>TESTTTTTEGPECSSWLGYCQVTDQCCRDLVCMGLYAKCVPGKIVDDNRPKGKGPFPPGN</t>
-  </si>
-  <si>
-    <t>TESTTTTTAPSYENSKAVCTPWLGYCQLTDQCCRDLICLTYAAKCVPGKIIDDKRPIGDGPFPPTGK</t>
-  </si>
-  <si>
-    <t>TESTTTTTETQQCSPWLQLCHVKEDCCRYLECSTYQAKCVPQSGLIIPGRDKRPLGPGPYPPNVPKEYLEE</t>
+    <t>TTEESSTTSCFKRNRQCKGSFLKSACCEGLKCVNGRCT</t>
+  </si>
+  <si>
+    <t>TTEESSTTDCCFSSSCRCNLWGSNCQCQRMGLFQKWGASPL</t>
+  </si>
+  <si>
+    <t>TTEESSTTCSPPGFFCQTDDDCCFTKLFRCLEIVGRCVKRNVTVASTTALPTNSINL</t>
+  </si>
+  <si>
+    <t>TTEESSTTSAIPHCSPWRCQQECLFKNFMKGECIQLQCVCSQKIGGIRP</t>
+  </si>
+  <si>
+    <t>TTEESSTTDCTGWMGGCDPSKTGECCSGYVCSYKYPWCRYDLF</t>
+  </si>
+  <si>
+    <t>TTEESSTTVSFCLLPIVPGPCTQYVIRYAFQPSISACRRFTFGGCEGNDNNFMTRRDCEHYCEELL</t>
+  </si>
+  <si>
+    <t>TTEESSTTYKGCRRLGSKCHPTLKPCCSALTCKPIDGDNGECVE</t>
+  </si>
+  <si>
+    <t>TTEESSTTYCLGSGEECGKFDDCCSLTCMSNGECA</t>
+  </si>
+  <si>
+    <t>TTEESSTTCSPPGAVCDSFNNCCTGFMCNPWAKRCTRGFFDRIPLKTKKYNFSNQIMNEE</t>
+  </si>
+  <si>
+    <t>TTEESSTTAPNSMDSCFDLAQFCVMSEQCCPGLQCSSYAAKCIPIYIYN</t>
+  </si>
+  <si>
+    <t>TTEESSTTEGPECSSWLGYCQVTDQCCRDLVCMGLYAKCVPGKIVDDNRPKGKGPFPPGN</t>
+  </si>
+  <si>
+    <t>TTEESSTTAPSYENSKAVCTPWLGYCQLTDQCCRDLICLTYAAKCVPGKIIDDKRPIGDGPFPPTGK</t>
+  </si>
+  <si>
+    <t>TTEESSTTETQQCSPWLQLCHVKEDCCRYLECSTYQAKCVPQSGLIIPGRDKRPLGPGPYPPNVPKEYLEE</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>